<commit_message>
atualizao layout, incluido app marketplace, ajustado o model do app product, ajustado arquivos statics
</commit_message>
<xml_diff>
--- a/data/lista-produtos-full.xlsx
+++ b/data/lista-produtos-full.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenie\Documents\Python Scripts\hackathon-poatek\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F3211F-6C73-47ED-BB6B-25A72A75F61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7D3E13-EA21-46D5-89B8-CF4E20DA2BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{1B8EAF27-DBCB-43BF-8835-F66F7E6B3978}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{1B8EAF27-DBCB-43BF-8835-F66F7E6B3978}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="256">
   <si>
     <t>Nissin</t>
   </si>
@@ -747,13 +748,70 @@
   </si>
   <si>
     <t>Farofa mandioca. Farofa pronta. Para melhor conservação das características do produto, mantenha-o fechado após o uso</t>
+  </si>
+  <si>
+    <t>massas</t>
+  </si>
+  <si>
+    <t>categoria</t>
+  </si>
+  <si>
+    <t>Gãos</t>
+  </si>
+  <si>
+    <t>condor</t>
+  </si>
+  <si>
+    <t>extra</t>
+  </si>
+  <si>
+    <t>pão de açucar</t>
+  </si>
+  <si>
+    <t>Biscoitos, salgadinhos e snacks</t>
+  </si>
+  <si>
+    <t>Carnes e aves</t>
+  </si>
+  <si>
+    <t>Congelados</t>
+  </si>
+  <si>
+    <t>Básico da despensa</t>
+  </si>
+  <si>
+    <t>Doces e sobremesas</t>
+  </si>
+  <si>
+    <t>Enlatados e conservas</t>
+  </si>
+  <si>
+    <t>Frios</t>
+  </si>
+  <si>
+    <t>Molhos, temperos e condimentos</t>
+  </si>
+  <si>
+    <t>Padaria e confeitaria</t>
+  </si>
+  <si>
+    <t>Peixaria</t>
+  </si>
+  <si>
+    <t>Queijos e laticínios</t>
+  </si>
+  <si>
+    <t>Sementes e oleaginosas</t>
+  </si>
+  <si>
+    <t>Fruas, legumes e verduras</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -766,6 +824,13 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -788,12 +853,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1108,1107 +1174,1216 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D381464-8C2D-4837-B765-5713752C9B0F}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="194.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="194.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2">
+        <v>9.9</v>
+      </c>
+      <c r="C2">
+        <v>10.8</v>
+      </c>
+      <c r="D2">
+        <v>13.1</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B3">
+        <v>0.99</v>
+      </c>
+      <c r="C3">
+        <v>1.5</v>
+      </c>
+      <c r="D3">
+        <v>1.8</v>
+      </c>
+      <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="H3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F3" t="s">
+      <c r="J3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B4">
+        <v>2.89</v>
+      </c>
+      <c r="C4">
+        <v>3.1</v>
+      </c>
+      <c r="D4">
+        <v>3.49</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C4" t="s">
+      <c r="G4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="H4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
+      <c r="I4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s">
+      <c r="J4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B5">
+        <v>2.99</v>
+      </c>
+      <c r="C5">
+        <v>3.45</v>
+      </c>
+      <c r="D5">
+        <v>3.9</v>
+      </c>
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="H5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
+      <c r="I5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" t="s">
+      <c r="J5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>237</v>
+      </c>
+      <c r="B6">
+        <v>15.02</v>
+      </c>
+      <c r="C6">
+        <v>16.25</v>
+      </c>
+      <c r="D6">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="E6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C6" t="s">
+      <c r="G6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
+      <c r="H6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" t="s">
+      <c r="I6" t="s">
         <v>22</v>
       </c>
-      <c r="F6" t="s">
+      <c r="J6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C7" t="s">
+      <c r="G7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s">
+      <c r="H7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" t="s">
+      <c r="I7" t="s">
         <v>25</v>
       </c>
-      <c r="F7" t="s">
+      <c r="J7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C8" t="s">
+      <c r="G8" t="s">
         <v>30</v>
       </c>
-      <c r="D8" t="s">
+      <c r="H8" t="s">
         <v>31</v>
       </c>
-      <c r="E8" t="s">
+      <c r="I8" t="s">
         <v>0</v>
       </c>
-      <c r="F8" t="s">
+      <c r="J8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C9" t="s">
+      <c r="G9" t="s">
         <v>33</v>
       </c>
-      <c r="D9" t="s">
+      <c r="H9" t="s">
         <v>32</v>
       </c>
-      <c r="E9" t="s">
+      <c r="I9" t="s">
         <v>22</v>
       </c>
-      <c r="F9" t="s">
+      <c r="J9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C10" t="s">
+      <c r="G10" t="s">
         <v>36</v>
       </c>
-      <c r="D10" t="s">
+      <c r="H10" t="s">
         <v>39</v>
       </c>
-      <c r="E10" t="s">
+      <c r="I10" t="s">
         <v>37</v>
       </c>
-      <c r="F10" t="s">
+      <c r="J10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C11" t="s">
+      <c r="G11" t="s">
         <v>41</v>
       </c>
-      <c r="D11" t="s">
+      <c r="H11" t="s">
         <v>44</v>
       </c>
-      <c r="E11" t="s">
+      <c r="I11" t="s">
         <v>42</v>
       </c>
-      <c r="F11" t="s">
+      <c r="J11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C12" t="s">
+      <c r="G12" t="s">
         <v>46</v>
       </c>
-      <c r="D12" t="s">
+      <c r="H12" t="s">
         <v>47</v>
       </c>
-      <c r="E12" t="s">
+      <c r="I12" t="s">
         <v>48</v>
       </c>
-      <c r="F12" t="s">
+      <c r="J12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C13" t="s">
+      <c r="G13" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="E13" t="s">
+      <c r="I13" t="s">
         <v>51</v>
       </c>
-      <c r="F13" t="s">
+      <c r="J13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C14" t="s">
+      <c r="G14" t="s">
         <v>149</v>
       </c>
-      <c r="D14" t="s">
+      <c r="H14" t="s">
         <v>56</v>
       </c>
-      <c r="E14" t="s">
+      <c r="I14" t="s">
         <v>54</v>
       </c>
-      <c r="F14" t="s">
+      <c r="J14" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C15" t="s">
+      <c r="G15" t="s">
         <v>59</v>
       </c>
-      <c r="D15" t="s">
+      <c r="H15" t="s">
         <v>60</v>
       </c>
-      <c r="E15" t="s">
+      <c r="I15" t="s">
         <v>42</v>
       </c>
-      <c r="F15" t="s">
+      <c r="J15" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C16" t="s">
+      <c r="G16" t="s">
         <v>63</v>
       </c>
-      <c r="D16" t="s">
+      <c r="H16" t="s">
         <v>62</v>
       </c>
-      <c r="E16" t="s">
+      <c r="I16" t="s">
         <v>48</v>
       </c>
-      <c r="F16" t="s">
+      <c r="J16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C17" t="s">
+      <c r="G17" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E17" t="s">
+      <c r="I17" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C18" t="s">
+      <c r="G18" t="s">
         <v>21</v>
       </c>
-      <c r="D18" t="s">
+      <c r="H18" t="s">
         <v>72</v>
       </c>
-      <c r="E18" t="s">
+      <c r="I18" t="s">
         <v>70</v>
       </c>
-      <c r="F18" t="s">
+      <c r="J18" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C19" t="s">
+      <c r="G19" t="s">
         <v>46</v>
       </c>
-      <c r="D19" t="s">
+      <c r="H19" t="s">
         <v>75</v>
       </c>
-      <c r="E19" t="s">
+      <c r="I19" t="s">
         <v>37</v>
       </c>
-      <c r="F19" t="s">
+      <c r="J19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>239</v>
+      </c>
+      <c r="B20">
+        <v>4.99</v>
+      </c>
+      <c r="C20">
+        <v>5.8</v>
+      </c>
+      <c r="D20">
+        <v>6.12</v>
+      </c>
+      <c r="E20" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C20" t="s">
+      <c r="G20" t="s">
         <v>77</v>
       </c>
-      <c r="D20" t="s">
+      <c r="H20" t="s">
         <v>78</v>
       </c>
-      <c r="E20" t="s">
+      <c r="I20" t="s">
         <v>79</v>
       </c>
-      <c r="F20" t="s">
+      <c r="J20" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>239</v>
+      </c>
+      <c r="B21">
+        <v>5.8</v>
+      </c>
+      <c r="C21">
+        <v>6.3</v>
+      </c>
+      <c r="D21">
+        <v>6.89</v>
+      </c>
+      <c r="E21" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C21" t="s">
+      <c r="G21" t="s">
         <v>77</v>
       </c>
-      <c r="D21" t="s">
+      <c r="H21" t="s">
         <v>78</v>
       </c>
-      <c r="E21" t="s">
+      <c r="I21" t="s">
         <v>82</v>
       </c>
-      <c r="F21" t="s">
+      <c r="J21" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C22" t="s">
+      <c r="G22" t="s">
         <v>148</v>
       </c>
-      <c r="D22" t="s">
+      <c r="H22" t="s">
         <v>84</v>
       </c>
-      <c r="E22" t="s">
+      <c r="I22" t="s">
         <v>48</v>
       </c>
-      <c r="F22" t="s">
+      <c r="J22" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
         <v>86</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C23" t="s">
+      <c r="G23" t="s">
         <v>87</v>
       </c>
-      <c r="D23" t="s">
+      <c r="H23" t="s">
         <v>88</v>
       </c>
-      <c r="E23" t="s">
+      <c r="I23" t="s">
         <v>25</v>
       </c>
-      <c r="F23" t="s">
+      <c r="J23" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="C24" t="s">
+      <c r="G24" t="s">
         <v>91</v>
       </c>
-      <c r="D24" t="s">
+      <c r="H24" t="s">
         <v>92</v>
       </c>
-      <c r="E24" t="s">
+      <c r="I24" t="s">
         <v>17</v>
       </c>
-      <c r="F24" t="s">
+      <c r="J24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
         <v>93</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C25" t="s">
+      <c r="G25" t="s">
         <v>91</v>
       </c>
-      <c r="D25" t="s">
+      <c r="H25" t="s">
         <v>94</v>
       </c>
-      <c r="E25" t="s">
+      <c r="I25" t="s">
         <v>17</v>
       </c>
-      <c r="F25" t="s">
+      <c r="J25" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
         <v>95</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C26" t="s">
+      <c r="G26" t="s">
         <v>91</v>
       </c>
-      <c r="D26" t="s">
+      <c r="H26" t="s">
         <v>94</v>
       </c>
-      <c r="E26" t="s">
+      <c r="I26" t="s">
         <v>17</v>
       </c>
-      <c r="F26" t="s">
+      <c r="J26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
         <v>96</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C27" t="s">
+      <c r="G27" t="s">
         <v>46</v>
       </c>
-      <c r="D27" t="s">
+      <c r="H27" t="s">
         <v>97</v>
       </c>
-      <c r="E27" t="s">
+      <c r="I27" t="s">
         <v>98</v>
       </c>
-      <c r="F27" t="s">
+      <c r="J27" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>239</v>
+      </c>
+      <c r="B28">
+        <v>3.89</v>
+      </c>
+      <c r="C28">
+        <v>3.99</v>
+      </c>
+      <c r="D28">
+        <v>4.8</v>
+      </c>
+      <c r="E28" t="s">
         <v>99</v>
       </c>
-      <c r="C28" t="s">
+      <c r="G28" t="s">
         <v>77</v>
       </c>
-      <c r="D28" t="s">
+      <c r="H28" t="s">
         <v>101</v>
       </c>
-      <c r="E28" t="s">
+      <c r="I28" t="s">
         <v>100</v>
       </c>
-      <c r="F28" t="s">
+      <c r="J28" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
         <v>102</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C29" t="s">
+      <c r="G29" t="s">
         <v>77</v>
       </c>
-      <c r="D29" t="s">
+      <c r="H29" t="s">
         <v>101</v>
       </c>
-      <c r="E29" t="s">
+      <c r="I29" t="s">
         <v>103</v>
       </c>
-      <c r="F29" t="s">
+      <c r="J29" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
         <v>104</v>
       </c>
-      <c r="C30" t="s">
+      <c r="G30" t="s">
         <v>77</v>
       </c>
-      <c r="D30" t="s">
+      <c r="H30" t="s">
         <v>106</v>
       </c>
-      <c r="E30" t="s">
+      <c r="I30" t="s">
         <v>105</v>
       </c>
-      <c r="F30" t="s">
+      <c r="J30" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
         <v>107</v>
       </c>
-      <c r="C31" t="s">
+      <c r="G31" t="s">
         <v>77</v>
       </c>
-      <c r="D31" t="s">
+      <c r="H31" t="s">
         <v>108</v>
       </c>
-      <c r="E31" t="s">
+      <c r="I31" t="s">
         <v>109</v>
       </c>
-      <c r="F31" t="s">
+      <c r="J31" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
         <v>110</v>
       </c>
-      <c r="C32" t="s">
+      <c r="G32" t="s">
         <v>77</v>
       </c>
-      <c r="D32" t="s">
+      <c r="H32" t="s">
         <v>101</v>
       </c>
-      <c r="E32" t="s">
+      <c r="I32" t="s">
         <v>111</v>
       </c>
-      <c r="F32" t="s">
+      <c r="J32" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
         <v>112</v>
       </c>
-      <c r="B33" t="s">
+      <c r="F33" t="s">
         <v>113</v>
       </c>
-      <c r="C33" t="s">
+      <c r="G33" t="s">
         <v>77</v>
       </c>
-      <c r="D33" t="s">
+      <c r="H33" t="s">
         <v>114</v>
       </c>
-      <c r="E33" t="s">
+      <c r="I33" t="s">
         <v>115</v>
       </c>
-      <c r="F33" t="s">
+      <c r="J33" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="34" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
         <v>116</v>
       </c>
-      <c r="B34" t="s">
+      <c r="F34" t="s">
         <v>117</v>
       </c>
-      <c r="C34" t="s">
+      <c r="G34" t="s">
         <v>77</v>
       </c>
-      <c r="D34" t="s">
+      <c r="H34" t="s">
         <v>114</v>
       </c>
-      <c r="E34" t="s">
+      <c r="I34" t="s">
         <v>115</v>
       </c>
-      <c r="F34" t="s">
+      <c r="J34" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="35" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
         <v>118</v>
       </c>
-      <c r="B35" t="s">
+      <c r="F35" t="s">
         <v>119</v>
       </c>
-      <c r="C35" t="s">
+      <c r="G35" t="s">
         <v>77</v>
       </c>
-      <c r="D35" t="s">
+      <c r="H35" t="s">
         <v>114</v>
       </c>
-      <c r="E35" t="s">
+      <c r="I35" t="s">
         <v>115</v>
       </c>
-      <c r="F35" t="s">
+      <c r="J35" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="36" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
         <v>120</v>
       </c>
-      <c r="B36" t="s">
+      <c r="F36" t="s">
         <v>121</v>
       </c>
-      <c r="C36" t="s">
+      <c r="G36" t="s">
         <v>77</v>
       </c>
-      <c r="D36" t="s">
+      <c r="H36" t="s">
         <v>114</v>
       </c>
-      <c r="E36" t="s">
+      <c r="I36" t="s">
         <v>122</v>
       </c>
-      <c r="F36" t="s">
+      <c r="J36" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="37" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
         <v>123</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C37" t="s">
+      <c r="G37" t="s">
         <v>127</v>
       </c>
-      <c r="D37" t="s">
+      <c r="H37" t="s">
         <v>126</v>
       </c>
-      <c r="E37" t="s">
+      <c r="I37" t="s">
         <v>125</v>
       </c>
-      <c r="F37" t="s">
+      <c r="J37" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
         <v>128</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C38" t="s">
+      <c r="G38" t="s">
         <v>129</v>
       </c>
-      <c r="D38" t="s">
+      <c r="H38" t="s">
         <v>130</v>
       </c>
-      <c r="E38" t="s">
+      <c r="I38" t="s">
         <v>25</v>
       </c>
-      <c r="F38" t="s">
+      <c r="J38" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="39" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
         <v>131</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C39" t="s">
+      <c r="G39" t="s">
         <v>132</v>
       </c>
-      <c r="D39" t="s">
+      <c r="H39" t="s">
         <v>133</v>
       </c>
-      <c r="E39" t="s">
+      <c r="I39" t="s">
         <v>25</v>
       </c>
-      <c r="F39" t="s">
+      <c r="J39" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="40" spans="5:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
         <v>134</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C40" t="s">
+      <c r="G40" t="s">
         <v>150</v>
       </c>
-      <c r="D40" t="s">
+      <c r="H40" t="s">
         <v>135</v>
       </c>
-      <c r="E40" t="s">
+      <c r="I40" t="s">
         <v>136</v>
       </c>
-      <c r="F40" t="s">
+      <c r="J40" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="41" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
         <v>138</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C41" t="s">
+      <c r="G41" t="s">
         <v>139</v>
       </c>
-      <c r="D41" t="s">
+      <c r="H41" t="s">
         <v>141</v>
       </c>
-      <c r="E41" t="s">
+      <c r="I41" t="s">
         <v>42</v>
       </c>
-      <c r="F41" t="s">
+      <c r="J41" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="42" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
         <v>142</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C42" t="s">
+      <c r="G42" t="s">
         <v>143</v>
       </c>
-      <c r="D42" t="s">
+      <c r="H42" t="s">
         <v>133</v>
       </c>
-      <c r="E42" t="s">
+      <c r="I42" t="s">
         <v>25</v>
       </c>
-      <c r="F42" t="s">
+      <c r="J42" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="43" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
         <v>144</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C43" t="s">
+      <c r="G43" t="s">
         <v>148</v>
       </c>
-      <c r="D43" t="s">
+      <c r="H43" t="s">
         <v>147</v>
       </c>
-      <c r="E43" t="s">
+      <c r="I43" t="s">
         <v>145</v>
       </c>
-      <c r="F43" t="s">
+      <c r="J43" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="44" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
         <v>151</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C44" t="s">
+      <c r="G44" t="s">
         <v>152</v>
       </c>
-      <c r="D44" t="s">
+      <c r="H44" t="s">
         <v>155</v>
       </c>
-      <c r="E44" t="s">
+      <c r="I44" t="s">
         <v>153</v>
       </c>
-      <c r="F44" t="s">
+      <c r="J44" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="45" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
         <v>156</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C45" t="s">
+      <c r="G45" t="s">
         <v>139</v>
       </c>
-      <c r="D45" t="s">
+      <c r="H45" t="s">
         <v>141</v>
       </c>
-      <c r="E45" t="s">
+      <c r="I45" t="s">
         <v>25</v>
       </c>
-      <c r="F45" t="s">
+      <c r="J45" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="46" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
         <v>158</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C46" t="s">
+      <c r="G46" t="s">
         <v>148</v>
       </c>
-      <c r="D46" t="s">
+      <c r="H46" t="s">
         <v>159</v>
       </c>
-      <c r="E46" t="s">
+      <c r="I46" t="s">
         <v>160</v>
       </c>
-      <c r="F46" t="s">
+      <c r="J46" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="47" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
         <v>162</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="F47" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C47" t="s">
+      <c r="G47" t="s">
         <v>163</v>
       </c>
-      <c r="D47" t="s">
+      <c r="H47" t="s">
         <v>164</v>
       </c>
-      <c r="E47" t="s">
+      <c r="I47" t="s">
         <v>165</v>
       </c>
-      <c r="F47" t="s">
+      <c r="J47" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="48" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
         <v>166</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C48" t="s">
+      <c r="G48" t="s">
         <v>21</v>
       </c>
-      <c r="D48" t="s">
+      <c r="H48" t="s">
         <v>167</v>
       </c>
-      <c r="E48" t="s">
+      <c r="I48" t="s">
         <v>168</v>
       </c>
-      <c r="F48" t="s">
+      <c r="J48" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="49" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
         <v>170</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="C49" t="s">
+      <c r="G49" t="s">
         <v>171</v>
       </c>
-      <c r="D49" t="s">
+      <c r="H49" t="s">
         <v>167</v>
       </c>
-      <c r="E49" t="s">
+      <c r="I49" t="s">
         <v>168</v>
       </c>
-      <c r="F49" t="s">
+      <c r="J49" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="50" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
         <v>172</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="F50" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C50" t="s">
+      <c r="G50" t="s">
         <v>21</v>
       </c>
-      <c r="D50" t="s">
+      <c r="H50" t="s">
         <v>173</v>
       </c>
-      <c r="E50" t="s">
+      <c r="I50" t="s">
         <v>168</v>
       </c>
-      <c r="F50" t="s">
+      <c r="J50" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="51" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
         <v>174</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C51" t="s">
+      <c r="G51" t="s">
         <v>175</v>
       </c>
-      <c r="D51" t="s">
+      <c r="H51" t="s">
         <v>176</v>
       </c>
-      <c r="E51" t="s">
+      <c r="I51" t="s">
         <v>177</v>
       </c>
-      <c r="F51" t="s">
+      <c r="J51" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="52" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
         <v>179</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="F52" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C52" t="s">
+      <c r="G52" t="s">
         <v>180</v>
       </c>
-      <c r="D52" t="s">
+      <c r="H52" t="s">
         <v>181</v>
       </c>
-      <c r="E52" t="s">
+      <c r="I52" t="s">
         <v>168</v>
       </c>
-      <c r="F52" t="s">
+      <c r="J52" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="53" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
         <v>182</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="F53" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C53" t="s">
+      <c r="G53" t="s">
         <v>183</v>
       </c>
-      <c r="D53" t="s">
+      <c r="H53" t="s">
         <v>184</v>
       </c>
-      <c r="E53" t="s">
+      <c r="I53" t="s">
         <v>186</v>
       </c>
-      <c r="F53" t="s">
+      <c r="J53" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="54" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
         <v>187</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C54" t="s">
+      <c r="G54" t="s">
         <v>188</v>
       </c>
-      <c r="D54" t="s">
+      <c r="H54" t="s">
         <v>189</v>
       </c>
-      <c r="E54" t="s">
+      <c r="I54" t="s">
         <v>168</v>
       </c>
-      <c r="F54" t="s">
+      <c r="J54" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="55" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
         <v>190</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="F55" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C55" t="s">
+      <c r="G55" t="s">
         <v>77</v>
       </c>
-      <c r="D55" t="s">
+      <c r="H55" t="s">
         <v>191</v>
       </c>
-      <c r="E55" t="s">
+      <c r="I55" t="s">
         <v>192</v>
       </c>
-      <c r="F55" t="s">
+      <c r="J55" t="s">
         <v>193</v>
       </c>
     </row>
@@ -2216,4 +2391,87 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE20D2E-D1E6-4FD3-9732-735763763B7B}">
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>254</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>